<commit_message>
removed old synthetic volume tests
</commit_message>
<xml_diff>
--- a/analysis/segthy_volumetrics_csa_summary.xlsx
+++ b/analysis/segthy_volumetrics_csa_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\catalyst-tools\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9F97C9F-69B8-4030-9C76-B7E8CCA63E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{C3CDF868-156A-48CC-8570-8A247BA30C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C38F0002-AC39-4C98-8787-A19F3F756503}"/>
   </bookViews>
@@ -874,7 +874,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -883,6 +883,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="7" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4184,13 +4187,17 @@
   <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+      <selection activeCell="Q64" sqref="Q64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="55" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="55" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -6768,22 +6775,22 @@
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+      <c r="A67" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="6">
         <v>3</v>
       </c>
-      <c r="D67" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="5">
+      <c r="D67" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7">
         <v>2.1877757252981902</v>
       </c>
-      <c r="F67" s="5">
+      <c r="F67" s="7">
         <v>41.451733333333301</v>
       </c>
       <c r="G67" s="5">
@@ -6885,22 +6892,22 @@
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="A70" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="6">
         <v>3</v>
       </c>
-      <c r="D70" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="5">
+      <c r="D70" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="7">
         <v>1.77810496876876</v>
       </c>
-      <c r="F70" s="5">
+      <c r="F70" s="7">
         <v>48.554526315789403</v>
       </c>
       <c r="G70" s="5">
@@ -7002,22 +7009,22 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+      <c r="A73" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="6">
         <v>5</v>
       </c>
-      <c r="D73" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="5">
+      <c r="D73" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E73" s="7">
         <v>0.81065658564123699</v>
       </c>
-      <c r="F73" s="5">
+      <c r="F73" s="7">
         <v>52.0703999999999</v>
       </c>
       <c r="G73" s="5">
@@ -7119,22 +7126,22 @@
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+      <c r="A76" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="6">
         <v>3</v>
       </c>
-      <c r="D76" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="5">
+      <c r="D76" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="7">
         <v>2.3695579654809098</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="7">
         <v>57.118628571428502</v>
       </c>
       <c r="G76" s="5">
@@ -7236,22 +7243,22 @@
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+      <c r="A79" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="6">
         <v>5</v>
       </c>
-      <c r="D79" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="5">
+      <c r="D79" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="7">
         <v>3.2462966143188301</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F79" s="7">
         <v>62.762879999999903</v>
       </c>
       <c r="G79" s="5">
@@ -7353,22 +7360,22 @@
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="A82" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="6">
         <v>5</v>
       </c>
-      <c r="D82" t="b">
-        <v>1</v>
-      </c>
-      <c r="E82" s="5">
+      <c r="D82" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7">
         <v>3.2448433664162799</v>
       </c>
-      <c r="F82" s="5">
+      <c r="F82" s="7">
         <v>62.813333333333297</v>
       </c>
       <c r="G82" s="5">
@@ -7470,22 +7477,22 @@
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+      <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="6">
         <v>5</v>
       </c>
-      <c r="D85" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" s="5">
+      <c r="D85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" s="7">
         <v>2.3941801274576999</v>
       </c>
-      <c r="F85" s="5">
+      <c r="F85" s="7">
         <v>64.967563636363593</v>
       </c>
       <c r="G85" s="5">
@@ -7660,22 +7667,22 @@
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="A90" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="6">
         <v>3</v>
       </c>
-      <c r="D90" t="b">
-        <v>1</v>
-      </c>
-      <c r="E90" s="5">
+      <c r="D90" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" s="7">
         <v>3.9704063257634901</v>
       </c>
-      <c r="F90" s="5">
+      <c r="F90" s="7">
         <v>78.980914285714206</v>
       </c>
       <c r="G90" s="5">
@@ -7777,22 +7784,22 @@
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="A93" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="6">
         <v>5</v>
       </c>
-      <c r="D93" t="b">
-        <v>1</v>
-      </c>
-      <c r="E93" s="5">
+      <c r="D93" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E93" s="7">
         <v>5.6265322155361401</v>
       </c>
-      <c r="F93" s="5">
+      <c r="F93" s="7">
         <v>86.378823529411704</v>
       </c>
       <c r="G93" s="5">
@@ -7894,22 +7901,22 @@
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+      <c r="A96" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="6">
         <v>5</v>
       </c>
-      <c r="D96" t="b">
-        <v>1</v>
-      </c>
-      <c r="E96" s="4">
+      <c r="D96" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E96" s="8">
         <v>4.4200941036095802</v>
       </c>
-      <c r="F96" s="5">
+      <c r="F96" s="7">
         <v>102.680639999999</v>
       </c>
       <c r="G96" s="5">

</xml_diff>